<commit_message>
Mise à jour des résultats du script
</commit_message>
<xml_diff>
--- a/result/Data.xlsx
+++ b/result/Data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -562,13 +562,29 @@
           <t>Rien ne nous concerne aujourd'hui !</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
+      <c r="C8" t="inlineStr"/>
       <c r="D8" t="n">
         <v>210</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-02-21</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Rien ne nous concerne aujourd'hui !</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>552</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Màj manuelle + correctifs
</commit_message>
<xml_diff>
--- a/result/Data.xlsx
+++ b/result/Data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,7 +468,7 @@
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="n">
-        <v>116</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -484,13 +484,13 @@
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
-        <v>116</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-02-19</t>
+          <t>2025-02-20</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -500,7 +500,7 @@
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
-        <v>116</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -516,13 +516,13 @@
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="n">
-        <v>210</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-02-20</t>
+          <t>2025-02-21</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -532,13 +532,13 @@
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="n">
-        <v>210</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-02-20</t>
+          <t>2025-02-24</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -548,13 +548,13 @@
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="n">
-        <v>210</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-02-20</t>
+          <t>2025-02-25</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -564,55 +564,61 @@
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="n">
-        <v>210</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-02-21</t>
+          <t>2025-02-26</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Rien ne nous concerne aujourd'hui !</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr"/>
+          <t>autorisation</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
       <c r="D9" t="n">
-        <v>552</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-02-24</t>
+          <t>2025-02-26</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Rien ne nous concerne aujourd'hui !</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr"/>
+          <t>service</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
       <c r="D10" t="n">
-        <v>234</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-02-25</t>
+          <t>2025-02-26</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Rien ne nous concerne aujourd'hui !</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr"/>
+          <t>service</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>2</v>
+      </c>
       <c r="D11" t="n">
-        <v>112</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12">
@@ -627,7 +633,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" t="n">
         <v>1</v>
@@ -641,14 +647,14 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>service</t>
+          <t>gouvernement</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -663,10 +669,10 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15">
@@ -677,11 +683,11 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>autorisation</t>
+          <t>gouvernement</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D15" t="n">
         <v>1</v>
@@ -695,14 +701,14 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>gouvernement</t>
+          <t>service</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17">
@@ -713,14 +719,14 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>service</t>
+          <t>autorisation</t>
         </is>
       </c>
       <c r="C17" t="n">
+        <v>5</v>
+      </c>
+      <c r="D17" t="n">
         <v>3</v>
-      </c>
-      <c r="D17" t="n">
-        <v>6</v>
       </c>
     </row>
     <row r="18">
@@ -731,14 +737,14 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>gouvernement</t>
+          <t>service</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D18" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19">
@@ -753,10 +759,10 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D19" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20">
@@ -767,11 +773,11 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>autorisation</t>
+          <t>service</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D20" t="n">
         <v>3</v>
@@ -789,10 +795,10 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D21" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22">
@@ -803,14 +809,14 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>service</t>
+          <t>autorisation</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D22" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23">
@@ -821,11 +827,11 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>service</t>
+          <t>gouvernement</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D23" t="n">
         <v>3</v>
@@ -843,10 +849,10 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
@@ -857,14 +863,14 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>autorisation</t>
+          <t>gouvernement</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D25" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26">
@@ -875,16 +881,14 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Rien ne nous concerne aujourd'hui !</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
+          <t>service</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>14</v>
       </c>
       <c r="D26" t="n">
-        <v>49</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -895,14 +899,14 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>gouvernement</t>
+          <t>autorisation</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D27" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -917,7 +921,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D28" t="n">
         <v>2</v>
@@ -931,11 +935,11 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>gouvernement</t>
+          <t>service</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D29" t="n">
         <v>7</v>
@@ -953,10 +957,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D30" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31">
@@ -967,14 +971,14 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>autorisation</t>
+          <t>service</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D31" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32">
@@ -989,7 +993,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D32" t="n">
         <v>2</v>
@@ -1007,10 +1011,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D33" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34">
@@ -1025,10 +1029,10 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D34" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35">
@@ -1043,10 +1047,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D35" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36">
@@ -1061,10 +1065,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D36" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37">
@@ -1079,10 +1083,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D37" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38">
@@ -1097,7 +1101,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D38" t="n">
         <v>3</v>
@@ -1115,10 +1119,10 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D39" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40">
@@ -1133,10 +1137,10 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D40" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
@@ -1151,81 +1155,9 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D41" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>2025-02-26</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>service</t>
-        </is>
-      </c>
-      <c r="C42" t="n">
-        <v>31</v>
-      </c>
-      <c r="D42" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>2025-02-26</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>service</t>
-        </is>
-      </c>
-      <c r="C43" t="n">
-        <v>32</v>
-      </c>
-      <c r="D43" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>2025-02-26</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>service</t>
-        </is>
-      </c>
-      <c r="C44" t="n">
-        <v>33</v>
-      </c>
-      <c r="D44" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>2025-02-26</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>service</t>
-        </is>
-      </c>
-      <c r="C45" t="n">
-        <v>34</v>
-      </c>
-      <c r="D45" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>